<commit_message>
Update sample Excel file
</commit_message>
<xml_diff>
--- a/Sample/meta-tag-analyzer-report.xlsx
+++ b/Sample/meta-tag-analyzer-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>URL</t>
   </si>
@@ -31,27 +31,36 @@
     <t>Meta title</t>
   </si>
   <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Open-graph image</t>
+  </si>
+  <si>
+    <t>Open-graph URL</t>
+  </si>
+  <si>
+    <t>Open-graph title</t>
+  </si>
+  <si>
+    <t>Open-graph title length</t>
+  </si>
+  <si>
+    <t>Open-graph description</t>
+  </si>
+  <si>
+    <t>Open-graph description length</t>
+  </si>
+  <si>
     <t>Open-graph type</t>
   </si>
   <si>
-    <t>Open-graph URL</t>
-  </si>
-  <si>
-    <t>Open-graph title</t>
-  </si>
-  <si>
-    <t>Open-graph title length</t>
-  </si>
-  <si>
-    <t>Open-graph description</t>
-  </si>
-  <si>
-    <t>Open-graph description length</t>
-  </si>
-  <si>
     <t>Site name</t>
   </si>
   <si>
+    <t>Language</t>
+  </si>
+  <si>
     <t>Twitter card type</t>
   </si>
   <si>
@@ -67,6 +76,18 @@
     <t>Facebook app ID</t>
   </si>
   <si>
+    <t>Robots meta tag</t>
+  </si>
+  <si>
+    <t>H1 element</t>
+  </si>
+  <si>
+    <t>H1 length</t>
+  </si>
+  <si>
+    <t>Number of H1 tags found</t>
+  </si>
+  <si>
     <t>https://profilesticker.net/</t>
   </si>
   <si>
@@ -76,10 +97,21 @@
     <t>Add a sticker to your profile picture using Profile Sticker in just 4 easy steps to reflect how you're feeling today, something new and interesting or maybe anything just for fun.</t>
   </si>
   <si>
+    <t>Profile Sticker, profile photo, profile overlay, Clyde D'Souza, web app, open source, fun stuff, add a sticker to my profile picture, create sticker, profile picture, upload from Facebook, post picture to Facebook, 
+          add new stickers, contribute, GitHub, stand out from the crowd, feature me, tag profile sticker, follow us on Facebook, follow us on Twitter, follow us on Instagram, follow us on YouTube, follow us on Google+, follow us on LinkedIn, Auckland, New Zealand, AKL, NZ, 
+          profilesticker.net, profile sticker .net, design institutes, home page, index, online portfolio, online profile, design a sticker</t>
+  </si>
+  <si>
+    <t>https://static.profilesticker.net/images/psassets/site-teaser-fresh.png</t>
+  </si>
+  <si>
+    <t>Add a sticker to your profile picture using Profile Sticker to reflect how you're feeling today, something new and interesting or maybe anything just for fun.</t>
+  </si>
+  <si>
     <t>website</t>
   </si>
   <si>
-    <t>Add a sticker to your profile picture using Profile Sticker to reflect how you're feeling today, something new and interesting or maybe anything just for fun.</t>
+    <t>en_US</t>
   </si>
   <si>
     <t>summary</t>
@@ -91,6 +123,9 @@
     <t>653803501477017</t>
   </si>
   <si>
+    <t>Profile Sticker - Add a sticker to your profile picture in just 4 easy steps</t>
+  </si>
+  <si>
     <t>https://recipybot.azurewebsites.net/About</t>
   </si>
   <si>
@@ -100,6 +135,12 @@
     <t>The Recipy Bot is your virtual friend who can assist you with selecting delicious recipes based on your requirements or ingredients on hand.</t>
   </si>
   <si>
+    <t>bot, facebook, skype, recipe, the recipy bot, orange, fruits, vegetables, meat, flat design, flat bot, orange bot</t>
+  </si>
+  <si>
+    <t>https://recipybot.azurewebsites.net/Images/banners/recipybot-site-teaser.png</t>
+  </si>
+  <si>
     <t>https://recipybot.azurewebsites.net</t>
   </si>
   <si>
@@ -109,6 +150,9 @@
     <t>1513642785395264</t>
   </si>
   <si>
+    <t>&lt;a href="/"&gt;The Recipy Bot&lt;/a&gt;</t>
+  </si>
+  <si>
     <t>https://clydedz.github.io/sass-snippet-pack/</t>
   </si>
   <si>
@@ -118,9 +162,18 @@
     <t>Sass Snippet Pack is a Visual Studio Extension to help you write scss code developed by Clyde D'Souza. Compatible with Visual Studio 2019. Download Now.</t>
   </si>
   <si>
+    <t>sass, scss, snippet pack, Clyde D'souza, visual studio, visual studio extension, visual studio marketplace, visual studio 2017, visual studio 2019, visual studio community, visual studio professional, visual studio enterprise</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ClydeDz/sass-snippet-pack/master/SassVsixExtension.Website/SassVsixExtension.Website/images/banners/sass-vsix-ext-siteteaser.png</t>
+  </si>
+  <si>
     <t>1189872997782304</t>
   </si>
   <si>
+    <t>Sass Snippet Pack</t>
+  </si>
+  <si>
     <t>https://clydedz.github.io/fancy-comments/</t>
   </si>
   <si>
@@ -130,9 +183,18 @@
     <t>Fancy Comments is a Visual Studio Extension for use-case specific comments, supported for HTML, CSS, JavaScript, C#, SQL and XML. Download Now.</t>
   </si>
   <si>
+    <t>csharp, c#, sql, css, html, xml, fancy, comments, snippet pack, Clyde D'souza, visual studio, visual studio extension, visual studio marketplace, visual studio 2017, visual studio 2019, visual studio 2015,visual studio 2013, visual studio 2012, visual studio community, visual studio professional, visual studio enterprise, clide</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ClydeDz/fancy-comments/master/docs/FancyComments.Web/images/banners/vsix-ext-siteteaser.png</t>
+  </si>
+  <si>
     <t>1592574260862002</t>
   </si>
   <si>
+    <t>Fancy Comments</t>
+  </si>
+  <si>
     <t>Legend:</t>
   </si>
   <si>
@@ -142,7 +204,13 @@
     <t>No data when required</t>
   </si>
   <si>
-    <t>Report geneted on:</t>
+    <t>Blank cells mean the tag wasn't found on a page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report generated on: </t>
+  </si>
+  <si>
+    <t>Tue Apr 30 2019 07:29:50 GMT+0000 (Coordinated Universal Time)</t>
   </si>
   <si>
     <t>Meta Tag Analyzer (c) 2019 Clyde D'Souza</t>
@@ -207,13 +275,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:Y13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,222 +678,320 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3">
         <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>179</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="3">
         <v>76</v>
       </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2">
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2">
         <v>158</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="3">
+        <v>76</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E3">
         <v>140</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3">
         <v>140</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3">
         <v>30</v>
       </c>
-      <c r="R3" t="s">
-        <v>31</v>
+      <c r="Y3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3">
         <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>152</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="3">
+        <v>62</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4">
+        <v>152</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" t="s">
+      <c r="Q4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="3">
-        <v>62</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4">
-        <v>152</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>30</v>
-      </c>
       <c r="R4" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="T4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4">
+        <v>17</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>143</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5">
         <v>59</v>
       </c>
-      <c r="K5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5">
+      <c r="L5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5">
         <v>143</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="R5" t="s">
-        <v>39</v>
+        <v>53</v>
+      </c>
+      <c r="T5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" t="s">
+        <v>58</v>
+      </c>
+      <c r="W5" t="s">
+        <v>59</v>
+      </c>
+      <c r="X5">
+        <v>14</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="5">
-        <v>43583.28410377315</v>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>